<commit_message>
new excel and re change keys
</commit_message>
<xml_diff>
--- a/spotifyusernames.xlsx
+++ b/spotifyusernames.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="289">
   <si>
     <t>Usernames</t>
   </si>
@@ -716,6 +716,45 @@
   </si>
   <si>
     <t>lucyspec26</t>
+  </si>
+  <si>
+    <t>lilpopsisdead</t>
+  </si>
+  <si>
+    <t>pkudv4sb28zc27l59irvfo73m</t>
+  </si>
+  <si>
+    <t>annissarep</t>
+  </si>
+  <si>
+    <t>ashstoneman10</t>
+  </si>
+  <si>
+    <t>jamie708</t>
+  </si>
+  <si>
+    <t>dypylk0iy3jhkc62sgt3l3qsr</t>
+  </si>
+  <si>
+    <t>bwoodrum1341</t>
+  </si>
+  <si>
+    <t>basherthegreat</t>
+  </si>
+  <si>
+    <t>premmamehta</t>
+  </si>
+  <si>
+    <t>kissane1</t>
+  </si>
+  <si>
+    <t>moonpearlium</t>
+  </si>
+  <si>
+    <t>314k2w7t3bwhqg57i5eox44icy4u</t>
+  </si>
+  <si>
+    <t>skeil5</t>
   </si>
   <si>
     <t>akeerthy</t>
@@ -851,7 +890,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -877,6 +916,10 @@
       <name val="Inconsolata"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -896,16 +939,30 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <right/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -943,8 +1000,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2582,293 +2645,332 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="2"/>
+      <c r="A233" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"lilpopsisdead")</f>
+        <v>lilpopsisdead</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"pkudv4sb28zc27l59irvfo73m")</f>
+        <v>pkudv4sb28zc27l59irvfo73m</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"annissarep")</f>
+        <v>annissarep</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ashstoneman10")</f>
+        <v>ashstoneman10</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"jamie708")</f>
+        <v>jamie708</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"dypylk0iy3jhkc62sgt3l3qsr")</f>
+        <v>dypylk0iy3jhkc62sgt3l3qsr</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"bwoodrum1341")</f>
+        <v>bwoodrum1341</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"basherthegreat")</f>
+        <v>basherthegreat</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"premmamehta")</f>
+        <v>premmamehta</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"kissane1")</f>
+        <v>kissane1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"moonpearlium")</f>
+        <v>moonpearlium</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"314k2w7t3bwhqg57i5eox44icy4u")</f>
+        <v>314k2w7t3bwhqg57i5eox44icy4u</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"skeil5")</f>
+        <v>skeil5</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Claudia.hastings0717")</f>
         <v>Claudia.hastings0717</v>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" s="2" t="str">
+    <row r="248">
+      <c r="A248" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"seapanda02")</f>
         <v>seapanda02</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" s="2" t="str">
+    <row r="249">
+      <c r="A249" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"minto45")</f>
         <v>minto45</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" s="2" t="str">
+    <row r="250">
+      <c r="A250" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"lbrockwell3")</f>
         <v>lbrockwell3</v>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" s="2" t="str">
+    <row r="251">
+      <c r="A251" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"sht6dz4j702fbpbi0bsdcpjbu")</f>
         <v>sht6dz4j702fbpbi0bsdcpjbu</v>
       </c>
     </row>
-    <row r="239">
-      <c r="A239" s="2" t="str">
+    <row r="252">
+      <c r="A252" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"417T6uUZED6VM8euKbFDnM")</f>
         <v>417T6uUZED6VM8euKbFDnM</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" s="2" t="str">
+    <row r="253">
+      <c r="A253" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ryguy829")</f>
         <v>ryguy829</v>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" s="2" t="str">
+    <row r="254">
+      <c r="A254" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"5g6wujia2mpdz49g9ifskqmt8")</f>
         <v>5g6wujia2mpdz49g9ifskqmt8</v>
       </c>
     </row>
-    <row r="242">
-      <c r="A242" s="2" t="str">
+    <row r="255">
+      <c r="A255" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ashleydiazdl")</f>
         <v>ashleydiazdl</v>
       </c>
     </row>
-    <row r="243">
-      <c r="A243" s="2" t="str">
+    <row r="256">
+      <c r="A256" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"2m91c7srplu1xe9q5ca5xk8fk")</f>
         <v>2m91c7srplu1xe9q5ca5xk8fk</v>
       </c>
     </row>
-    <row r="244">
-      <c r="A244" s="2" t="str">
+    <row r="257">
+      <c r="A257" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"cinnamon122")</f>
         <v>cinnamon122</v>
       </c>
     </row>
-    <row r="245">
-      <c r="A245" s="2" t="str">
+    <row r="258">
+      <c r="A258" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"graceshapiro1903")</f>
         <v>graceshapiro1903</v>
       </c>
     </row>
-    <row r="246">
-      <c r="A246" s="2" t="str">
+    <row r="259">
+      <c r="A259" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"dizxi4lkttkiyprdepck004y4")</f>
         <v>dizxi4lkttkiyprdepck004y4</v>
       </c>
     </row>
-    <row r="247">
-      <c r="A247" s="2" t="str">
+    <row r="260">
+      <c r="A260" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"cole_wolf16")</f>
         <v>cole_wolf16</v>
       </c>
     </row>
-    <row r="248">
-      <c r="A248" s="2" t="str">
+    <row r="261">
+      <c r="A261" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"quinnrennell")</f>
         <v>quinnrennell</v>
       </c>
     </row>
-    <row r="249">
-      <c r="A249" s="2" t="str">
+    <row r="262">
+      <c r="A262" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"dominatork")</f>
         <v>dominatork</v>
       </c>
     </row>
-    <row r="250">
-      <c r="A250" s="2" t="str">
+    <row r="263">
+      <c r="A263" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"spamjcooper3459")</f>
         <v>spamjcooper3459</v>
       </c>
     </row>
-    <row r="251">
-      <c r="A251" s="2" t="str">
+    <row r="264">
+      <c r="A264" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"5z5uf9efaqg4b9cr5eiku8rdv")</f>
         <v>5z5uf9efaqg4b9cr5eiku8rdv</v>
       </c>
     </row>
-    <row r="252">
-      <c r="A252" s="2" t="str">
+    <row r="265">
+      <c r="A265" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"22jmljvsabjrtfn3676bpqjpy")</f>
         <v>22jmljvsabjrtfn3676bpqjpy</v>
       </c>
     </row>
-    <row r="253">
-      <c r="A253" s="2" t="str">
+    <row r="266">
+      <c r="A266" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"mzarouk")</f>
         <v>mzarouk</v>
       </c>
     </row>
-    <row r="254">
-      <c r="A254" s="2" t="str">
+    <row r="267">
+      <c r="A267" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"adelsoneric")</f>
         <v>adelsoneric</v>
       </c>
     </row>
-    <row r="255">
-      <c r="A255" s="2" t="str">
+    <row r="268">
+      <c r="A268" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"6912zox87iu176v3oyoeq0zna")</f>
         <v>6912zox87iu176v3oyoeq0zna</v>
       </c>
     </row>
-    <row r="256">
-      <c r="A256" s="2" t="str">
+    <row r="269">
+      <c r="A269" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"sbalewlij5gpqkgpucb9jhdy5")</f>
         <v>sbalewlij5gpqkgpucb9jhdy5</v>
       </c>
     </row>
-    <row r="257">
-      <c r="A257" s="3" t="str">
+    <row r="270">
+      <c r="A270" s="3" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"olivia.ma")</f>
         <v>olivia.ma</v>
       </c>
     </row>
-    <row r="258">
-      <c r="A258" s="2" t="str">
+    <row r="271">
+      <c r="A271" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"sabrinasugg")</f>
         <v>sabrinasugg</v>
       </c>
     </row>
-    <row r="259">
-      <c r="A259" s="2" t="str">
+    <row r="272">
+      <c r="A272" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"memzwith1z")</f>
         <v>memzwith1z</v>
       </c>
     </row>
-    <row r="260">
-      <c r="A260" s="2" t="str">
+    <row r="273">
+      <c r="A273" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"a98x1imc6m4r4yrd0hz86h092")</f>
         <v>a98x1imc6m4r4yrd0hz86h092</v>
       </c>
     </row>
-    <row r="261">
-      <c r="A261" s="2" t="str">
+    <row r="274">
+      <c r="A274" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"carlygeezle")</f>
         <v>carlygeezle</v>
       </c>
     </row>
-    <row r="262">
-      <c r="A262" s="2" t="str">
+    <row r="275">
+      <c r="A275" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"tavoduvall")</f>
         <v>tavoduvall</v>
       </c>
     </row>
-    <row r="263">
-      <c r="A263" s="2" t="str">
+    <row r="276">
+      <c r="A276" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"9be7zye8x3t7dhi8jc03mfkye")</f>
         <v>9be7zye8x3t7dhi8jc03mfkye</v>
       </c>
     </row>
-    <row r="264">
-      <c r="A264" s="2" t="str">
+    <row r="277">
+      <c r="A277" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"bumbleebeebee2017")</f>
         <v>bumbleebeebee2017</v>
       </c>
     </row>
-    <row r="265">
-      <c r="A265" s="2" t="str">
+    <row r="278">
+      <c r="A278" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"curlyq013")</f>
         <v>curlyq013</v>
       </c>
     </row>
-    <row r="266">
-      <c r="A266" s="2" t="str">
+    <row r="279">
+      <c r="A279" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"d4503rf1nw1arbnrza08pbjyy")</f>
         <v>d4503rf1nw1arbnrza08pbjyy</v>
       </c>
     </row>
-    <row r="267">
-      <c r="A267" s="2" t="str">
+    <row r="280">
+      <c r="A280" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"dancingpuppydawg")</f>
         <v>dancingpuppydawg</v>
       </c>
     </row>
-    <row r="268">
-      <c r="A268" s="2" t="str">
+    <row r="281">
+      <c r="A281" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"martybaseball15")</f>
         <v>martybaseball15</v>
       </c>
     </row>
-    <row r="269">
-      <c r="A269" s="2" t="str">
+    <row r="282">
+      <c r="A282" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"masterchiqui")</f>
         <v>masterchiqui</v>
       </c>
     </row>
-    <row r="270">
-      <c r="A270" s="2" t="str">
+    <row r="283">
+      <c r="A283" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"ohur7tcdvhcigpuuqi9eofkcn")</f>
         <v>ohur7tcdvhcigpuuqi9eofkcn</v>
       </c>
     </row>
-    <row r="271">
-      <c r="A271" s="2" t="str">
+    <row r="284">
+      <c r="A284" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"rhea12344")</f>
         <v>rhea12344</v>
       </c>
     </row>
-    <row r="272">
-      <c r="A272" s="2" t="str">
+    <row r="285">
+      <c r="A285" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"thebeautyqueen98")</f>
         <v>thebeautyqueen98</v>
       </c>
     </row>
-    <row r="273">
-      <c r="A273" s="2" t="str">
+    <row r="286">
+      <c r="A286" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boolovesme")</f>
         <v>boolovesme</v>
       </c>
     </row>
-    <row r="274">
-      <c r="A274" s="2" t="str">
+    <row r="287">
+      <c r="A287" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"pranaygup12")</f>
         <v>pranaygup12</v>
       </c>
     </row>
-    <row r="275">
-      <c r="A275" s="2"/>
-    </row>
-    <row r="276">
-      <c r="A276" s="2"/>
-    </row>
-    <row r="277">
-      <c r="A277" s="2"/>
-    </row>
-    <row r="278">
-      <c r="A278" s="2"/>
-    </row>
-    <row r="279">
-      <c r="A279" s="2"/>
-    </row>
-    <row r="280">
-      <c r="A280" s="2"/>
-    </row>
-    <row r="281">
-      <c r="A281" s="2"/>
-    </row>
-    <row r="282">
-      <c r="A282" s="2"/>
-    </row>
-    <row r="283">
-      <c r="A283" s="2"/>
-    </row>
-    <row r="284">
-      <c r="A284" s="2"/>
-    </row>
-    <row r="285">
-      <c r="A285" s="2"/>
-    </row>
-    <row r="286">
-      <c r="A286" s="2"/>
-    </row>
-    <row r="287">
-      <c r="A287" s="2"/>
-    </row>
     <row r="288">
       <c r="A288" s="2"/>
     </row>
@@ -6510,7 +6612,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A257"/>
+    <hyperlink r:id="rId1" ref="A270"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -7705,2302 +7807,2328 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="13"/>
+      <c r="A235" s="13" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="236">
-      <c r="A236" s="13"/>
+      <c r="A236" s="14" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="237">
-      <c r="A237" s="13"/>
+      <c r="A237" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="238">
-      <c r="A238" s="13"/>
+      <c r="A238" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="239">
-      <c r="A239" s="13"/>
+      <c r="A239" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="240">
-      <c r="A240" s="13"/>
+      <c r="A240" s="14" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="241">
-      <c r="A241" s="13"/>
+      <c r="A241" s="13" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="242">
-      <c r="A242" s="13"/>
+      <c r="A242" s="13" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="243">
-      <c r="A243" s="13"/>
+      <c r="A243" s="13" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="244">
-      <c r="A244" s="13"/>
+      <c r="A244" s="13" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="245">
-      <c r="A245" s="13"/>
+      <c r="A245" s="13" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="246">
-      <c r="A246" s="13"/>
+      <c r="A246" s="14" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="247">
-      <c r="A247" s="13"/>
+      <c r="A247" s="13" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="248">
-      <c r="A248" s="13"/>
+      <c r="A248" s="15"/>
     </row>
     <row r="249">
-      <c r="A249" s="13"/>
+      <c r="A249" s="15"/>
     </row>
     <row r="250">
-      <c r="A250" s="13"/>
+      <c r="A250" s="15"/>
     </row>
     <row r="251">
-      <c r="A251" s="13"/>
+      <c r="A251" s="15"/>
     </row>
     <row r="252">
-      <c r="A252" s="13"/>
+      <c r="A252" s="15"/>
     </row>
     <row r="253">
-      <c r="A253" s="13"/>
+      <c r="A253" s="15"/>
     </row>
     <row r="254">
-      <c r="A254" s="13"/>
+      <c r="A254" s="15"/>
     </row>
     <row r="255">
-      <c r="A255" s="13"/>
+      <c r="A255" s="15"/>
     </row>
     <row r="256">
-      <c r="A256" s="13"/>
+      <c r="A256" s="15"/>
     </row>
     <row r="257">
-      <c r="A257" s="13"/>
+      <c r="A257" s="15"/>
     </row>
     <row r="258">
-      <c r="A258" s="13"/>
+      <c r="A258" s="15"/>
     </row>
     <row r="259">
-      <c r="A259" s="13"/>
+      <c r="A259" s="15"/>
     </row>
     <row r="260">
-      <c r="A260" s="13"/>
+      <c r="A260" s="15"/>
     </row>
     <row r="261">
-      <c r="A261" s="13"/>
+      <c r="A261" s="15"/>
     </row>
     <row r="262">
-      <c r="A262" s="13"/>
+      <c r="A262" s="15"/>
     </row>
     <row r="263">
-      <c r="A263" s="13"/>
+      <c r="A263" s="15"/>
     </row>
     <row r="264">
-      <c r="A264" s="13"/>
+      <c r="A264" s="15"/>
     </row>
     <row r="265">
-      <c r="A265" s="13"/>
+      <c r="A265" s="15"/>
     </row>
     <row r="266">
-      <c r="A266" s="13"/>
+      <c r="A266" s="15"/>
     </row>
     <row r="267">
-      <c r="A267" s="13"/>
+      <c r="A267" s="15"/>
     </row>
     <row r="268">
-      <c r="A268" s="13"/>
+      <c r="A268" s="15"/>
     </row>
     <row r="269">
-      <c r="A269" s="13"/>
+      <c r="A269" s="15"/>
     </row>
     <row r="270">
-      <c r="A270" s="13"/>
+      <c r="A270" s="15"/>
     </row>
     <row r="271">
-      <c r="A271" s="13"/>
+      <c r="A271" s="15"/>
     </row>
     <row r="272">
-      <c r="A272" s="13"/>
+      <c r="A272" s="15"/>
     </row>
     <row r="273">
-      <c r="A273" s="13"/>
+      <c r="A273" s="15"/>
     </row>
     <row r="274">
-      <c r="A274" s="13"/>
+      <c r="A274" s="15"/>
     </row>
     <row r="275">
-      <c r="A275" s="13"/>
+      <c r="A275" s="15"/>
     </row>
     <row r="276">
-      <c r="A276" s="13"/>
+      <c r="A276" s="15"/>
     </row>
     <row r="277">
-      <c r="A277" s="13"/>
+      <c r="A277" s="15"/>
     </row>
     <row r="278">
-      <c r="A278" s="13"/>
+      <c r="A278" s="15"/>
     </row>
     <row r="279">
-      <c r="A279" s="13"/>
+      <c r="A279" s="15"/>
     </row>
     <row r="280">
-      <c r="A280" s="13"/>
+      <c r="A280" s="15"/>
     </row>
     <row r="281">
-      <c r="A281" s="13"/>
+      <c r="A281" s="15"/>
     </row>
     <row r="282">
-      <c r="A282" s="13"/>
+      <c r="A282" s="15"/>
     </row>
     <row r="283">
-      <c r="A283" s="13"/>
+      <c r="A283" s="15"/>
     </row>
     <row r="284">
-      <c r="A284" s="13"/>
+      <c r="A284" s="15"/>
     </row>
     <row r="285">
-      <c r="A285" s="13"/>
+      <c r="A285" s="15"/>
     </row>
     <row r="286">
-      <c r="A286" s="13"/>
+      <c r="A286" s="15"/>
     </row>
     <row r="287">
-      <c r="A287" s="13"/>
+      <c r="A287" s="15"/>
     </row>
     <row r="288">
-      <c r="A288" s="13"/>
+      <c r="A288" s="15"/>
     </row>
     <row r="289">
-      <c r="A289" s="13"/>
+      <c r="A289" s="15"/>
     </row>
     <row r="290">
-      <c r="A290" s="13"/>
+      <c r="A290" s="15"/>
     </row>
     <row r="291">
-      <c r="A291" s="13"/>
+      <c r="A291" s="15"/>
     </row>
     <row r="292">
-      <c r="A292" s="13"/>
+      <c r="A292" s="15"/>
     </row>
     <row r="293">
-      <c r="A293" s="13"/>
+      <c r="A293" s="15"/>
     </row>
     <row r="294">
-      <c r="A294" s="13"/>
+      <c r="A294" s="15"/>
     </row>
     <row r="295">
-      <c r="A295" s="13"/>
+      <c r="A295" s="15"/>
     </row>
     <row r="296">
-      <c r="A296" s="13"/>
+      <c r="A296" s="15"/>
     </row>
     <row r="297">
-      <c r="A297" s="13"/>
+      <c r="A297" s="15"/>
     </row>
     <row r="298">
-      <c r="A298" s="13"/>
+      <c r="A298" s="15"/>
     </row>
     <row r="299">
-      <c r="A299" s="13"/>
+      <c r="A299" s="15"/>
     </row>
     <row r="300">
-      <c r="A300" s="13"/>
+      <c r="A300" s="15"/>
     </row>
     <row r="301">
-      <c r="A301" s="13"/>
+      <c r="A301" s="15"/>
     </row>
     <row r="302">
-      <c r="A302" s="13"/>
+      <c r="A302" s="15"/>
     </row>
     <row r="303">
-      <c r="A303" s="13"/>
+      <c r="A303" s="15"/>
     </row>
     <row r="304">
-      <c r="A304" s="13"/>
+      <c r="A304" s="15"/>
     </row>
     <row r="305">
-      <c r="A305" s="13"/>
+      <c r="A305" s="15"/>
     </row>
     <row r="306">
-      <c r="A306" s="13"/>
+      <c r="A306" s="15"/>
     </row>
     <row r="307">
-      <c r="A307" s="13"/>
+      <c r="A307" s="15"/>
     </row>
     <row r="308">
-      <c r="A308" s="13"/>
+      <c r="A308" s="15"/>
     </row>
     <row r="309">
-      <c r="A309" s="13"/>
+      <c r="A309" s="15"/>
     </row>
     <row r="310">
-      <c r="A310" s="13"/>
+      <c r="A310" s="15"/>
     </row>
     <row r="311">
-      <c r="A311" s="13"/>
+      <c r="A311" s="15"/>
     </row>
     <row r="312">
-      <c r="A312" s="13"/>
+      <c r="A312" s="15"/>
     </row>
     <row r="313">
-      <c r="A313" s="13"/>
+      <c r="A313" s="15"/>
     </row>
     <row r="314">
-      <c r="A314" s="13"/>
+      <c r="A314" s="15"/>
     </row>
     <row r="315">
-      <c r="A315" s="13"/>
+      <c r="A315" s="15"/>
     </row>
     <row r="316">
-      <c r="A316" s="13"/>
+      <c r="A316" s="15"/>
     </row>
     <row r="317">
-      <c r="A317" s="13"/>
+      <c r="A317" s="15"/>
     </row>
     <row r="318">
-      <c r="A318" s="13"/>
+      <c r="A318" s="15"/>
     </row>
     <row r="319">
-      <c r="A319" s="13"/>
+      <c r="A319" s="15"/>
     </row>
     <row r="320">
-      <c r="A320" s="13"/>
+      <c r="A320" s="15"/>
     </row>
     <row r="321">
-      <c r="A321" s="13"/>
+      <c r="A321" s="15"/>
     </row>
     <row r="322">
-      <c r="A322" s="13"/>
+      <c r="A322" s="15"/>
     </row>
     <row r="323">
-      <c r="A323" s="13"/>
+      <c r="A323" s="15"/>
     </row>
     <row r="324">
-      <c r="A324" s="13"/>
+      <c r="A324" s="15"/>
     </row>
     <row r="325">
-      <c r="A325" s="13"/>
+      <c r="A325" s="15"/>
     </row>
     <row r="326">
-      <c r="A326" s="13"/>
+      <c r="A326" s="15"/>
     </row>
     <row r="327">
-      <c r="A327" s="13"/>
+      <c r="A327" s="15"/>
     </row>
     <row r="328">
-      <c r="A328" s="13"/>
+      <c r="A328" s="15"/>
     </row>
     <row r="329">
-      <c r="A329" s="13"/>
+      <c r="A329" s="15"/>
     </row>
     <row r="330">
-      <c r="A330" s="13"/>
+      <c r="A330" s="15"/>
     </row>
     <row r="331">
-      <c r="A331" s="13"/>
+      <c r="A331" s="15"/>
     </row>
     <row r="332">
-      <c r="A332" s="13"/>
+      <c r="A332" s="15"/>
     </row>
     <row r="333">
-      <c r="A333" s="13"/>
+      <c r="A333" s="15"/>
     </row>
     <row r="334">
-      <c r="A334" s="13"/>
+      <c r="A334" s="15"/>
     </row>
     <row r="335">
-      <c r="A335" s="13"/>
+      <c r="A335" s="15"/>
     </row>
     <row r="336">
-      <c r="A336" s="13"/>
+      <c r="A336" s="15"/>
     </row>
     <row r="337">
-      <c r="A337" s="13"/>
+      <c r="A337" s="15"/>
     </row>
     <row r="338">
-      <c r="A338" s="13"/>
+      <c r="A338" s="15"/>
     </row>
     <row r="339">
-      <c r="A339" s="13"/>
+      <c r="A339" s="15"/>
     </row>
     <row r="340">
-      <c r="A340" s="13"/>
+      <c r="A340" s="15"/>
     </row>
     <row r="341">
-      <c r="A341" s="13"/>
+      <c r="A341" s="15"/>
     </row>
     <row r="342">
-      <c r="A342" s="13"/>
+      <c r="A342" s="15"/>
     </row>
     <row r="343">
-      <c r="A343" s="13"/>
+      <c r="A343" s="15"/>
     </row>
     <row r="344">
-      <c r="A344" s="13"/>
+      <c r="A344" s="15"/>
     </row>
     <row r="345">
-      <c r="A345" s="13"/>
+      <c r="A345" s="15"/>
     </row>
     <row r="346">
-      <c r="A346" s="13"/>
+      <c r="A346" s="15"/>
     </row>
     <row r="347">
-      <c r="A347" s="13"/>
+      <c r="A347" s="15"/>
     </row>
     <row r="348">
-      <c r="A348" s="13"/>
+      <c r="A348" s="15"/>
     </row>
     <row r="349">
-      <c r="A349" s="13"/>
+      <c r="A349" s="15"/>
     </row>
     <row r="350">
-      <c r="A350" s="13"/>
+      <c r="A350" s="15"/>
     </row>
     <row r="351">
-      <c r="A351" s="13"/>
+      <c r="A351" s="15"/>
     </row>
     <row r="352">
-      <c r="A352" s="13"/>
+      <c r="A352" s="15"/>
     </row>
     <row r="353">
-      <c r="A353" s="13"/>
+      <c r="A353" s="15"/>
     </row>
     <row r="354">
-      <c r="A354" s="13"/>
+      <c r="A354" s="15"/>
     </row>
     <row r="355">
-      <c r="A355" s="13"/>
+      <c r="A355" s="15"/>
     </row>
     <row r="356">
-      <c r="A356" s="13"/>
+      <c r="A356" s="15"/>
     </row>
     <row r="357">
-      <c r="A357" s="13"/>
+      <c r="A357" s="15"/>
     </row>
     <row r="358">
-      <c r="A358" s="13"/>
+      <c r="A358" s="15"/>
     </row>
     <row r="359">
-      <c r="A359" s="13"/>
+      <c r="A359" s="15"/>
     </row>
     <row r="360">
-      <c r="A360" s="13"/>
+      <c r="A360" s="15"/>
     </row>
     <row r="361">
-      <c r="A361" s="13"/>
+      <c r="A361" s="15"/>
     </row>
     <row r="362">
-      <c r="A362" s="13"/>
+      <c r="A362" s="15"/>
     </row>
     <row r="363">
-      <c r="A363" s="13"/>
+      <c r="A363" s="15"/>
     </row>
     <row r="364">
-      <c r="A364" s="13"/>
+      <c r="A364" s="15"/>
     </row>
     <row r="365">
-      <c r="A365" s="13"/>
+      <c r="A365" s="15"/>
     </row>
     <row r="366">
-      <c r="A366" s="13"/>
+      <c r="A366" s="15"/>
     </row>
     <row r="367">
-      <c r="A367" s="13"/>
+      <c r="A367" s="15"/>
     </row>
     <row r="368">
-      <c r="A368" s="13"/>
+      <c r="A368" s="15"/>
     </row>
     <row r="369">
-      <c r="A369" s="13"/>
+      <c r="A369" s="15"/>
     </row>
     <row r="370">
-      <c r="A370" s="13"/>
+      <c r="A370" s="15"/>
     </row>
     <row r="371">
-      <c r="A371" s="13"/>
+      <c r="A371" s="15"/>
     </row>
     <row r="372">
-      <c r="A372" s="13"/>
+      <c r="A372" s="15"/>
     </row>
     <row r="373">
-      <c r="A373" s="13"/>
+      <c r="A373" s="15"/>
     </row>
     <row r="374">
-      <c r="A374" s="13"/>
+      <c r="A374" s="15"/>
     </row>
     <row r="375">
-      <c r="A375" s="13"/>
+      <c r="A375" s="15"/>
     </row>
     <row r="376">
-      <c r="A376" s="13"/>
+      <c r="A376" s="15"/>
     </row>
     <row r="377">
-      <c r="A377" s="13"/>
+      <c r="A377" s="15"/>
     </row>
     <row r="378">
-      <c r="A378" s="13"/>
+      <c r="A378" s="15"/>
     </row>
     <row r="379">
-      <c r="A379" s="13"/>
+      <c r="A379" s="15"/>
     </row>
     <row r="380">
-      <c r="A380" s="13"/>
+      <c r="A380" s="15"/>
     </row>
     <row r="381">
-      <c r="A381" s="13"/>
+      <c r="A381" s="15"/>
     </row>
     <row r="382">
-      <c r="A382" s="13"/>
+      <c r="A382" s="15"/>
     </row>
     <row r="383">
-      <c r="A383" s="13"/>
+      <c r="A383" s="15"/>
     </row>
     <row r="384">
-      <c r="A384" s="13"/>
+      <c r="A384" s="15"/>
     </row>
     <row r="385">
-      <c r="A385" s="13"/>
+      <c r="A385" s="15"/>
     </row>
     <row r="386">
-      <c r="A386" s="13"/>
+      <c r="A386" s="15"/>
     </row>
     <row r="387">
-      <c r="A387" s="13"/>
+      <c r="A387" s="15"/>
     </row>
     <row r="388">
-      <c r="A388" s="13"/>
+      <c r="A388" s="15"/>
     </row>
     <row r="389">
-      <c r="A389" s="13"/>
+      <c r="A389" s="15"/>
     </row>
     <row r="390">
-      <c r="A390" s="13"/>
+      <c r="A390" s="15"/>
     </row>
     <row r="391">
-      <c r="A391" s="13"/>
+      <c r="A391" s="15"/>
     </row>
     <row r="392">
-      <c r="A392" s="13"/>
+      <c r="A392" s="15"/>
     </row>
     <row r="393">
-      <c r="A393" s="13"/>
+      <c r="A393" s="15"/>
     </row>
     <row r="394">
-      <c r="A394" s="13"/>
+      <c r="A394" s="15"/>
     </row>
     <row r="395">
-      <c r="A395" s="13"/>
+      <c r="A395" s="15"/>
     </row>
     <row r="396">
-      <c r="A396" s="13"/>
+      <c r="A396" s="15"/>
     </row>
     <row r="397">
-      <c r="A397" s="13"/>
+      <c r="A397" s="15"/>
     </row>
     <row r="398">
-      <c r="A398" s="13"/>
+      <c r="A398" s="15"/>
     </row>
     <row r="399">
-      <c r="A399" s="13"/>
+      <c r="A399" s="15"/>
     </row>
     <row r="400">
-      <c r="A400" s="13"/>
+      <c r="A400" s="15"/>
     </row>
     <row r="401">
-      <c r="A401" s="13"/>
+      <c r="A401" s="15"/>
     </row>
     <row r="402">
-      <c r="A402" s="13"/>
+      <c r="A402" s="15"/>
     </row>
     <row r="403">
-      <c r="A403" s="13"/>
+      <c r="A403" s="15"/>
     </row>
     <row r="404">
-      <c r="A404" s="13"/>
+      <c r="A404" s="15"/>
     </row>
     <row r="405">
-      <c r="A405" s="13"/>
+      <c r="A405" s="15"/>
     </row>
     <row r="406">
-      <c r="A406" s="13"/>
+      <c r="A406" s="15"/>
     </row>
     <row r="407">
-      <c r="A407" s="13"/>
+      <c r="A407" s="15"/>
     </row>
     <row r="408">
-      <c r="A408" s="13"/>
+      <c r="A408" s="15"/>
     </row>
     <row r="409">
-      <c r="A409" s="13"/>
+      <c r="A409" s="15"/>
     </row>
     <row r="410">
-      <c r="A410" s="13"/>
+      <c r="A410" s="15"/>
     </row>
     <row r="411">
-      <c r="A411" s="13"/>
+      <c r="A411" s="15"/>
     </row>
     <row r="412">
-      <c r="A412" s="13"/>
+      <c r="A412" s="15"/>
     </row>
     <row r="413">
-      <c r="A413" s="13"/>
+      <c r="A413" s="15"/>
     </row>
     <row r="414">
-      <c r="A414" s="13"/>
+      <c r="A414" s="15"/>
     </row>
     <row r="415">
-      <c r="A415" s="13"/>
+      <c r="A415" s="15"/>
     </row>
     <row r="416">
-      <c r="A416" s="13"/>
+      <c r="A416" s="15"/>
     </row>
     <row r="417">
-      <c r="A417" s="13"/>
+      <c r="A417" s="15"/>
     </row>
     <row r="418">
-      <c r="A418" s="13"/>
+      <c r="A418" s="15"/>
     </row>
     <row r="419">
-      <c r="A419" s="13"/>
+      <c r="A419" s="15"/>
     </row>
     <row r="420">
-      <c r="A420" s="13"/>
+      <c r="A420" s="15"/>
     </row>
     <row r="421">
-      <c r="A421" s="13"/>
+      <c r="A421" s="15"/>
     </row>
     <row r="422">
-      <c r="A422" s="13"/>
+      <c r="A422" s="15"/>
     </row>
     <row r="423">
-      <c r="A423" s="13"/>
+      <c r="A423" s="15"/>
     </row>
     <row r="424">
-      <c r="A424" s="13"/>
+      <c r="A424" s="15"/>
     </row>
     <row r="425">
-      <c r="A425" s="13"/>
+      <c r="A425" s="15"/>
     </row>
     <row r="426">
-      <c r="A426" s="13"/>
+      <c r="A426" s="15"/>
     </row>
     <row r="427">
-      <c r="A427" s="13"/>
+      <c r="A427" s="15"/>
     </row>
     <row r="428">
-      <c r="A428" s="13"/>
+      <c r="A428" s="15"/>
     </row>
     <row r="429">
-      <c r="A429" s="13"/>
+      <c r="A429" s="15"/>
     </row>
     <row r="430">
-      <c r="A430" s="13"/>
+      <c r="A430" s="15"/>
     </row>
     <row r="431">
-      <c r="A431" s="13"/>
+      <c r="A431" s="15"/>
     </row>
     <row r="432">
-      <c r="A432" s="13"/>
+      <c r="A432" s="15"/>
     </row>
     <row r="433">
-      <c r="A433" s="13"/>
+      <c r="A433" s="15"/>
     </row>
     <row r="434">
-      <c r="A434" s="13"/>
+      <c r="A434" s="15"/>
     </row>
     <row r="435">
-      <c r="A435" s="13"/>
+      <c r="A435" s="15"/>
     </row>
     <row r="436">
-      <c r="A436" s="13"/>
+      <c r="A436" s="15"/>
     </row>
     <row r="437">
-      <c r="A437" s="13"/>
+      <c r="A437" s="15"/>
     </row>
     <row r="438">
-      <c r="A438" s="13"/>
+      <c r="A438" s="15"/>
     </row>
     <row r="439">
-      <c r="A439" s="13"/>
+      <c r="A439" s="15"/>
     </row>
     <row r="440">
-      <c r="A440" s="13"/>
+      <c r="A440" s="15"/>
     </row>
     <row r="441">
-      <c r="A441" s="13"/>
+      <c r="A441" s="15"/>
     </row>
     <row r="442">
-      <c r="A442" s="13"/>
+      <c r="A442" s="15"/>
     </row>
     <row r="443">
-      <c r="A443" s="13"/>
+      <c r="A443" s="15"/>
     </row>
     <row r="444">
-      <c r="A444" s="13"/>
+      <c r="A444" s="15"/>
     </row>
     <row r="445">
-      <c r="A445" s="13"/>
+      <c r="A445" s="15"/>
     </row>
     <row r="446">
-      <c r="A446" s="13"/>
+      <c r="A446" s="15"/>
     </row>
     <row r="447">
-      <c r="A447" s="13"/>
+      <c r="A447" s="15"/>
     </row>
     <row r="448">
-      <c r="A448" s="13"/>
+      <c r="A448" s="15"/>
     </row>
     <row r="449">
-      <c r="A449" s="13"/>
+      <c r="A449" s="15"/>
     </row>
     <row r="450">
-      <c r="A450" s="13"/>
+      <c r="A450" s="15"/>
     </row>
     <row r="451">
-      <c r="A451" s="13"/>
+      <c r="A451" s="15"/>
     </row>
     <row r="452">
-      <c r="A452" s="13"/>
+      <c r="A452" s="15"/>
     </row>
     <row r="453">
-      <c r="A453" s="13"/>
+      <c r="A453" s="15"/>
     </row>
     <row r="454">
-      <c r="A454" s="13"/>
+      <c r="A454" s="15"/>
     </row>
     <row r="455">
-      <c r="A455" s="13"/>
+      <c r="A455" s="15"/>
     </row>
     <row r="456">
-      <c r="A456" s="13"/>
+      <c r="A456" s="15"/>
     </row>
     <row r="457">
-      <c r="A457" s="13"/>
+      <c r="A457" s="15"/>
     </row>
     <row r="458">
-      <c r="A458" s="13"/>
+      <c r="A458" s="15"/>
     </row>
     <row r="459">
-      <c r="A459" s="13"/>
+      <c r="A459" s="15"/>
     </row>
     <row r="460">
-      <c r="A460" s="13"/>
+      <c r="A460" s="15"/>
     </row>
     <row r="461">
-      <c r="A461" s="13"/>
+      <c r="A461" s="15"/>
     </row>
     <row r="462">
-      <c r="A462" s="13"/>
+      <c r="A462" s="15"/>
     </row>
     <row r="463">
-      <c r="A463" s="13"/>
+      <c r="A463" s="15"/>
     </row>
     <row r="464">
-      <c r="A464" s="13"/>
+      <c r="A464" s="15"/>
     </row>
     <row r="465">
-      <c r="A465" s="13"/>
+      <c r="A465" s="15"/>
     </row>
     <row r="466">
-      <c r="A466" s="13"/>
+      <c r="A466" s="15"/>
     </row>
     <row r="467">
-      <c r="A467" s="13"/>
+      <c r="A467" s="15"/>
     </row>
     <row r="468">
-      <c r="A468" s="13"/>
+      <c r="A468" s="15"/>
     </row>
     <row r="469">
-      <c r="A469" s="13"/>
+      <c r="A469" s="15"/>
     </row>
     <row r="470">
-      <c r="A470" s="13"/>
+      <c r="A470" s="15"/>
     </row>
     <row r="471">
-      <c r="A471" s="13"/>
+      <c r="A471" s="15"/>
     </row>
     <row r="472">
-      <c r="A472" s="13"/>
+      <c r="A472" s="15"/>
     </row>
     <row r="473">
-      <c r="A473" s="13"/>
+      <c r="A473" s="15"/>
     </row>
     <row r="474">
-      <c r="A474" s="13"/>
+      <c r="A474" s="15"/>
     </row>
     <row r="475">
-      <c r="A475" s="13"/>
+      <c r="A475" s="15"/>
     </row>
     <row r="476">
-      <c r="A476" s="13"/>
+      <c r="A476" s="15"/>
     </row>
     <row r="477">
-      <c r="A477" s="13"/>
+      <c r="A477" s="15"/>
     </row>
     <row r="478">
-      <c r="A478" s="13"/>
+      <c r="A478" s="15"/>
     </row>
     <row r="479">
-      <c r="A479" s="13"/>
+      <c r="A479" s="15"/>
     </row>
     <row r="480">
-      <c r="A480" s="13"/>
+      <c r="A480" s="15"/>
     </row>
     <row r="481">
-      <c r="A481" s="13"/>
+      <c r="A481" s="15"/>
     </row>
     <row r="482">
-      <c r="A482" s="13"/>
+      <c r="A482" s="15"/>
     </row>
     <row r="483">
-      <c r="A483" s="13"/>
+      <c r="A483" s="15"/>
     </row>
     <row r="484">
-      <c r="A484" s="13"/>
+      <c r="A484" s="15"/>
     </row>
     <row r="485">
-      <c r="A485" s="13"/>
+      <c r="A485" s="15"/>
     </row>
     <row r="486">
-      <c r="A486" s="13"/>
+      <c r="A486" s="15"/>
     </row>
     <row r="487">
-      <c r="A487" s="13"/>
+      <c r="A487" s="15"/>
     </row>
     <row r="488">
-      <c r="A488" s="13"/>
+      <c r="A488" s="15"/>
     </row>
     <row r="489">
-      <c r="A489" s="13"/>
+      <c r="A489" s="15"/>
     </row>
     <row r="490">
-      <c r="A490" s="13"/>
+      <c r="A490" s="15"/>
     </row>
     <row r="491">
-      <c r="A491" s="13"/>
+      <c r="A491" s="15"/>
     </row>
     <row r="492">
-      <c r="A492" s="13"/>
+      <c r="A492" s="15"/>
     </row>
     <row r="493">
-      <c r="A493" s="13"/>
+      <c r="A493" s="15"/>
     </row>
     <row r="494">
-      <c r="A494" s="13"/>
+      <c r="A494" s="15"/>
     </row>
     <row r="495">
-      <c r="A495" s="13"/>
+      <c r="A495" s="15"/>
     </row>
     <row r="496">
-      <c r="A496" s="13"/>
+      <c r="A496" s="15"/>
     </row>
     <row r="497">
-      <c r="A497" s="13"/>
+      <c r="A497" s="15"/>
     </row>
     <row r="498">
-      <c r="A498" s="13"/>
+      <c r="A498" s="15"/>
     </row>
     <row r="499">
-      <c r="A499" s="13"/>
+      <c r="A499" s="15"/>
     </row>
     <row r="500">
-      <c r="A500" s="13"/>
+      <c r="A500" s="15"/>
     </row>
     <row r="501">
-      <c r="A501" s="13"/>
+      <c r="A501" s="15"/>
     </row>
     <row r="502">
-      <c r="A502" s="13"/>
+      <c r="A502" s="15"/>
     </row>
     <row r="503">
-      <c r="A503" s="13"/>
+      <c r="A503" s="15"/>
     </row>
     <row r="504">
-      <c r="A504" s="13"/>
+      <c r="A504" s="15"/>
     </row>
     <row r="505">
-      <c r="A505" s="13"/>
+      <c r="A505" s="15"/>
     </row>
     <row r="506">
-      <c r="A506" s="13"/>
+      <c r="A506" s="15"/>
     </row>
     <row r="507">
-      <c r="A507" s="13"/>
+      <c r="A507" s="15"/>
     </row>
     <row r="508">
-      <c r="A508" s="13"/>
+      <c r="A508" s="15"/>
     </row>
     <row r="509">
-      <c r="A509" s="13"/>
+      <c r="A509" s="15"/>
     </row>
     <row r="510">
-      <c r="A510" s="13"/>
+      <c r="A510" s="15"/>
     </row>
     <row r="511">
-      <c r="A511" s="13"/>
+      <c r="A511" s="15"/>
     </row>
     <row r="512">
-      <c r="A512" s="13"/>
+      <c r="A512" s="15"/>
     </row>
     <row r="513">
-      <c r="A513" s="13"/>
+      <c r="A513" s="15"/>
     </row>
     <row r="514">
-      <c r="A514" s="13"/>
+      <c r="A514" s="15"/>
     </row>
     <row r="515">
-      <c r="A515" s="13"/>
+      <c r="A515" s="15"/>
     </row>
     <row r="516">
-      <c r="A516" s="13"/>
+      <c r="A516" s="15"/>
     </row>
     <row r="517">
-      <c r="A517" s="13"/>
+      <c r="A517" s="15"/>
     </row>
     <row r="518">
-      <c r="A518" s="13"/>
+      <c r="A518" s="15"/>
     </row>
     <row r="519">
-      <c r="A519" s="13"/>
+      <c r="A519" s="15"/>
     </row>
     <row r="520">
-      <c r="A520" s="13"/>
+      <c r="A520" s="15"/>
     </row>
     <row r="521">
-      <c r="A521" s="13"/>
+      <c r="A521" s="15"/>
     </row>
     <row r="522">
-      <c r="A522" s="13"/>
+      <c r="A522" s="15"/>
     </row>
     <row r="523">
-      <c r="A523" s="13"/>
+      <c r="A523" s="15"/>
     </row>
     <row r="524">
-      <c r="A524" s="13"/>
+      <c r="A524" s="15"/>
     </row>
     <row r="525">
-      <c r="A525" s="13"/>
+      <c r="A525" s="15"/>
     </row>
     <row r="526">
-      <c r="A526" s="13"/>
+      <c r="A526" s="15"/>
     </row>
     <row r="527">
-      <c r="A527" s="13"/>
+      <c r="A527" s="15"/>
     </row>
     <row r="528">
-      <c r="A528" s="13"/>
+      <c r="A528" s="15"/>
     </row>
     <row r="529">
-      <c r="A529" s="13"/>
+      <c r="A529" s="15"/>
     </row>
     <row r="530">
-      <c r="A530" s="13"/>
+      <c r="A530" s="15"/>
     </row>
     <row r="531">
-      <c r="A531" s="13"/>
+      <c r="A531" s="15"/>
     </row>
     <row r="532">
-      <c r="A532" s="13"/>
+      <c r="A532" s="15"/>
     </row>
     <row r="533">
-      <c r="A533" s="13"/>
+      <c r="A533" s="15"/>
     </row>
     <row r="534">
-      <c r="A534" s="13"/>
+      <c r="A534" s="15"/>
     </row>
     <row r="535">
-      <c r="A535" s="13"/>
+      <c r="A535" s="15"/>
     </row>
     <row r="536">
-      <c r="A536" s="13"/>
+      <c r="A536" s="15"/>
     </row>
     <row r="537">
-      <c r="A537" s="13"/>
+      <c r="A537" s="15"/>
     </row>
     <row r="538">
-      <c r="A538" s="13"/>
+      <c r="A538" s="15"/>
     </row>
     <row r="539">
-      <c r="A539" s="13"/>
+      <c r="A539" s="15"/>
     </row>
     <row r="540">
-      <c r="A540" s="13"/>
+      <c r="A540" s="15"/>
     </row>
     <row r="541">
-      <c r="A541" s="13"/>
+      <c r="A541" s="15"/>
     </row>
     <row r="542">
-      <c r="A542" s="13"/>
+      <c r="A542" s="15"/>
     </row>
     <row r="543">
-      <c r="A543" s="13"/>
+      <c r="A543" s="15"/>
     </row>
     <row r="544">
-      <c r="A544" s="13"/>
+      <c r="A544" s="15"/>
     </row>
     <row r="545">
-      <c r="A545" s="13"/>
+      <c r="A545" s="15"/>
     </row>
     <row r="546">
-      <c r="A546" s="13"/>
+      <c r="A546" s="15"/>
     </row>
     <row r="547">
-      <c r="A547" s="13"/>
+      <c r="A547" s="15"/>
     </row>
     <row r="548">
-      <c r="A548" s="13"/>
+      <c r="A548" s="15"/>
     </row>
     <row r="549">
-      <c r="A549" s="13"/>
+      <c r="A549" s="15"/>
     </row>
     <row r="550">
-      <c r="A550" s="13"/>
+      <c r="A550" s="15"/>
     </row>
     <row r="551">
-      <c r="A551" s="13"/>
+      <c r="A551" s="15"/>
     </row>
     <row r="552">
-      <c r="A552" s="13"/>
+      <c r="A552" s="15"/>
     </row>
     <row r="553">
-      <c r="A553" s="13"/>
+      <c r="A553" s="15"/>
     </row>
     <row r="554">
-      <c r="A554" s="13"/>
+      <c r="A554" s="15"/>
     </row>
     <row r="555">
-      <c r="A555" s="13"/>
+      <c r="A555" s="15"/>
     </row>
     <row r="556">
-      <c r="A556" s="13"/>
+      <c r="A556" s="15"/>
     </row>
     <row r="557">
-      <c r="A557" s="13"/>
+      <c r="A557" s="15"/>
     </row>
     <row r="558">
-      <c r="A558" s="13"/>
+      <c r="A558" s="15"/>
     </row>
     <row r="559">
-      <c r="A559" s="13"/>
+      <c r="A559" s="15"/>
     </row>
     <row r="560">
-      <c r="A560" s="13"/>
+      <c r="A560" s="15"/>
     </row>
     <row r="561">
-      <c r="A561" s="13"/>
+      <c r="A561" s="15"/>
     </row>
     <row r="562">
-      <c r="A562" s="13"/>
+      <c r="A562" s="15"/>
     </row>
     <row r="563">
-      <c r="A563" s="13"/>
+      <c r="A563" s="15"/>
     </row>
     <row r="564">
-      <c r="A564" s="13"/>
+      <c r="A564" s="15"/>
     </row>
     <row r="565">
-      <c r="A565" s="13"/>
+      <c r="A565" s="15"/>
     </row>
     <row r="566">
-      <c r="A566" s="13"/>
+      <c r="A566" s="15"/>
     </row>
     <row r="567">
-      <c r="A567" s="13"/>
+      <c r="A567" s="15"/>
     </row>
     <row r="568">
-      <c r="A568" s="13"/>
+      <c r="A568" s="15"/>
     </row>
     <row r="569">
-      <c r="A569" s="13"/>
+      <c r="A569" s="15"/>
     </row>
     <row r="570">
-      <c r="A570" s="13"/>
+      <c r="A570" s="15"/>
     </row>
     <row r="571">
-      <c r="A571" s="13"/>
+      <c r="A571" s="15"/>
     </row>
     <row r="572">
-      <c r="A572" s="13"/>
+      <c r="A572" s="15"/>
     </row>
     <row r="573">
-      <c r="A573" s="13"/>
+      <c r="A573" s="15"/>
     </row>
     <row r="574">
-      <c r="A574" s="13"/>
+      <c r="A574" s="15"/>
     </row>
     <row r="575">
-      <c r="A575" s="13"/>
+      <c r="A575" s="15"/>
     </row>
     <row r="576">
-      <c r="A576" s="13"/>
+      <c r="A576" s="15"/>
     </row>
     <row r="577">
-      <c r="A577" s="13"/>
+      <c r="A577" s="15"/>
     </row>
     <row r="578">
-      <c r="A578" s="13"/>
+      <c r="A578" s="15"/>
     </row>
     <row r="579">
-      <c r="A579" s="13"/>
+      <c r="A579" s="15"/>
     </row>
     <row r="580">
-      <c r="A580" s="13"/>
+      <c r="A580" s="15"/>
     </row>
     <row r="581">
-      <c r="A581" s="13"/>
+      <c r="A581" s="15"/>
     </row>
     <row r="582">
-      <c r="A582" s="13"/>
+      <c r="A582" s="15"/>
     </row>
     <row r="583">
-      <c r="A583" s="13"/>
+      <c r="A583" s="15"/>
     </row>
     <row r="584">
-      <c r="A584" s="13"/>
+      <c r="A584" s="15"/>
     </row>
     <row r="585">
-      <c r="A585" s="13"/>
+      <c r="A585" s="15"/>
     </row>
     <row r="586">
-      <c r="A586" s="13"/>
+      <c r="A586" s="15"/>
     </row>
     <row r="587">
-      <c r="A587" s="13"/>
+      <c r="A587" s="15"/>
     </row>
     <row r="588">
-      <c r="A588" s="13"/>
+      <c r="A588" s="15"/>
     </row>
     <row r="589">
-      <c r="A589" s="13"/>
+      <c r="A589" s="15"/>
     </row>
     <row r="590">
-      <c r="A590" s="13"/>
+      <c r="A590" s="15"/>
     </row>
     <row r="591">
-      <c r="A591" s="13"/>
+      <c r="A591" s="15"/>
     </row>
     <row r="592">
-      <c r="A592" s="13"/>
+      <c r="A592" s="15"/>
     </row>
     <row r="593">
-      <c r="A593" s="13"/>
+      <c r="A593" s="15"/>
     </row>
     <row r="594">
-      <c r="A594" s="13"/>
+      <c r="A594" s="15"/>
     </row>
     <row r="595">
-      <c r="A595" s="13"/>
+      <c r="A595" s="15"/>
     </row>
     <row r="596">
-      <c r="A596" s="13"/>
+      <c r="A596" s="15"/>
     </row>
     <row r="597">
-      <c r="A597" s="13"/>
+      <c r="A597" s="15"/>
     </row>
     <row r="598">
-      <c r="A598" s="13"/>
+      <c r="A598" s="15"/>
     </row>
     <row r="599">
-      <c r="A599" s="13"/>
+      <c r="A599" s="15"/>
     </row>
     <row r="600">
-      <c r="A600" s="13"/>
+      <c r="A600" s="15"/>
     </row>
     <row r="601">
-      <c r="A601" s="13"/>
+      <c r="A601" s="15"/>
     </row>
     <row r="602">
-      <c r="A602" s="13"/>
+      <c r="A602" s="15"/>
     </row>
     <row r="603">
-      <c r="A603" s="13"/>
+      <c r="A603" s="15"/>
     </row>
     <row r="604">
-      <c r="A604" s="13"/>
+      <c r="A604" s="15"/>
     </row>
     <row r="605">
-      <c r="A605" s="13"/>
+      <c r="A605" s="15"/>
     </row>
     <row r="606">
-      <c r="A606" s="13"/>
+      <c r="A606" s="15"/>
     </row>
     <row r="607">
-      <c r="A607" s="13"/>
+      <c r="A607" s="15"/>
     </row>
     <row r="608">
-      <c r="A608" s="13"/>
+      <c r="A608" s="15"/>
     </row>
     <row r="609">
-      <c r="A609" s="13"/>
+      <c r="A609" s="15"/>
     </row>
     <row r="610">
-      <c r="A610" s="13"/>
+      <c r="A610" s="15"/>
     </row>
     <row r="611">
-      <c r="A611" s="13"/>
+      <c r="A611" s="15"/>
     </row>
     <row r="612">
-      <c r="A612" s="13"/>
+      <c r="A612" s="15"/>
     </row>
     <row r="613">
-      <c r="A613" s="13"/>
+      <c r="A613" s="15"/>
     </row>
     <row r="614">
-      <c r="A614" s="13"/>
+      <c r="A614" s="15"/>
     </row>
     <row r="615">
-      <c r="A615" s="13"/>
+      <c r="A615" s="15"/>
     </row>
     <row r="616">
-      <c r="A616" s="13"/>
+      <c r="A616" s="15"/>
     </row>
     <row r="617">
-      <c r="A617" s="13"/>
+      <c r="A617" s="15"/>
     </row>
     <row r="618">
-      <c r="A618" s="13"/>
+      <c r="A618" s="15"/>
     </row>
     <row r="619">
-      <c r="A619" s="13"/>
+      <c r="A619" s="15"/>
     </row>
     <row r="620">
-      <c r="A620" s="13"/>
+      <c r="A620" s="15"/>
     </row>
     <row r="621">
-      <c r="A621" s="13"/>
+      <c r="A621" s="15"/>
     </row>
     <row r="622">
-      <c r="A622" s="13"/>
+      <c r="A622" s="15"/>
     </row>
     <row r="623">
-      <c r="A623" s="13"/>
+      <c r="A623" s="15"/>
     </row>
     <row r="624">
-      <c r="A624" s="13"/>
+      <c r="A624" s="15"/>
     </row>
     <row r="625">
-      <c r="A625" s="13"/>
+      <c r="A625" s="15"/>
     </row>
     <row r="626">
-      <c r="A626" s="13"/>
+      <c r="A626" s="15"/>
     </row>
     <row r="627">
-      <c r="A627" s="13"/>
+      <c r="A627" s="15"/>
     </row>
     <row r="628">
-      <c r="A628" s="13"/>
+      <c r="A628" s="15"/>
     </row>
     <row r="629">
-      <c r="A629" s="13"/>
+      <c r="A629" s="15"/>
     </row>
     <row r="630">
-      <c r="A630" s="13"/>
+      <c r="A630" s="15"/>
     </row>
     <row r="631">
-      <c r="A631" s="13"/>
+      <c r="A631" s="15"/>
     </row>
     <row r="632">
-      <c r="A632" s="13"/>
+      <c r="A632" s="15"/>
     </row>
     <row r="633">
-      <c r="A633" s="13"/>
+      <c r="A633" s="15"/>
     </row>
     <row r="634">
-      <c r="A634" s="13"/>
+      <c r="A634" s="15"/>
     </row>
     <row r="635">
-      <c r="A635" s="13"/>
+      <c r="A635" s="15"/>
     </row>
     <row r="636">
-      <c r="A636" s="13"/>
+      <c r="A636" s="15"/>
     </row>
     <row r="637">
-      <c r="A637" s="13"/>
+      <c r="A637" s="15"/>
     </row>
     <row r="638">
-      <c r="A638" s="13"/>
+      <c r="A638" s="15"/>
     </row>
     <row r="639">
-      <c r="A639" s="13"/>
+      <c r="A639" s="15"/>
     </row>
     <row r="640">
-      <c r="A640" s="13"/>
+      <c r="A640" s="15"/>
     </row>
     <row r="641">
-      <c r="A641" s="13"/>
+      <c r="A641" s="15"/>
     </row>
     <row r="642">
-      <c r="A642" s="13"/>
+      <c r="A642" s="15"/>
     </row>
     <row r="643">
-      <c r="A643" s="13"/>
+      <c r="A643" s="15"/>
     </row>
     <row r="644">
-      <c r="A644" s="13"/>
+      <c r="A644" s="15"/>
     </row>
     <row r="645">
-      <c r="A645" s="13"/>
+      <c r="A645" s="15"/>
     </row>
     <row r="646">
-      <c r="A646" s="13"/>
+      <c r="A646" s="15"/>
     </row>
     <row r="647">
-      <c r="A647" s="13"/>
+      <c r="A647" s="15"/>
     </row>
     <row r="648">
-      <c r="A648" s="13"/>
+      <c r="A648" s="15"/>
     </row>
     <row r="649">
-      <c r="A649" s="13"/>
+      <c r="A649" s="15"/>
     </row>
     <row r="650">
-      <c r="A650" s="13"/>
+      <c r="A650" s="15"/>
     </row>
     <row r="651">
-      <c r="A651" s="13"/>
+      <c r="A651" s="15"/>
     </row>
     <row r="652">
-      <c r="A652" s="13"/>
+      <c r="A652" s="15"/>
     </row>
     <row r="653">
-      <c r="A653" s="13"/>
+      <c r="A653" s="15"/>
     </row>
     <row r="654">
-      <c r="A654" s="13"/>
+      <c r="A654" s="15"/>
     </row>
     <row r="655">
-      <c r="A655" s="13"/>
+      <c r="A655" s="15"/>
     </row>
     <row r="656">
-      <c r="A656" s="13"/>
+      <c r="A656" s="15"/>
     </row>
     <row r="657">
-      <c r="A657" s="13"/>
+      <c r="A657" s="15"/>
     </row>
     <row r="658">
-      <c r="A658" s="13"/>
+      <c r="A658" s="15"/>
     </row>
     <row r="659">
-      <c r="A659" s="13"/>
+      <c r="A659" s="15"/>
     </row>
     <row r="660">
-      <c r="A660" s="13"/>
+      <c r="A660" s="15"/>
     </row>
     <row r="661">
-      <c r="A661" s="13"/>
+      <c r="A661" s="15"/>
     </row>
     <row r="662">
-      <c r="A662" s="13"/>
+      <c r="A662" s="15"/>
     </row>
     <row r="663">
-      <c r="A663" s="13"/>
+      <c r="A663" s="15"/>
     </row>
     <row r="664">
-      <c r="A664" s="13"/>
+      <c r="A664" s="15"/>
     </row>
     <row r="665">
-      <c r="A665" s="13"/>
+      <c r="A665" s="15"/>
     </row>
     <row r="666">
-      <c r="A666" s="13"/>
+      <c r="A666" s="15"/>
     </row>
     <row r="667">
-      <c r="A667" s="13"/>
+      <c r="A667" s="15"/>
     </row>
     <row r="668">
-      <c r="A668" s="13"/>
+      <c r="A668" s="15"/>
     </row>
     <row r="669">
-      <c r="A669" s="13"/>
+      <c r="A669" s="15"/>
     </row>
     <row r="670">
-      <c r="A670" s="13"/>
+      <c r="A670" s="15"/>
     </row>
     <row r="671">
-      <c r="A671" s="13"/>
+      <c r="A671" s="15"/>
     </row>
     <row r="672">
-      <c r="A672" s="13"/>
+      <c r="A672" s="15"/>
     </row>
     <row r="673">
-      <c r="A673" s="13"/>
+      <c r="A673" s="15"/>
     </row>
     <row r="674">
-      <c r="A674" s="13"/>
+      <c r="A674" s="15"/>
     </row>
     <row r="675">
-      <c r="A675" s="13"/>
+      <c r="A675" s="15"/>
     </row>
     <row r="676">
-      <c r="A676" s="13"/>
+      <c r="A676" s="15"/>
     </row>
     <row r="677">
-      <c r="A677" s="13"/>
+      <c r="A677" s="15"/>
     </row>
     <row r="678">
-      <c r="A678" s="13"/>
+      <c r="A678" s="15"/>
     </row>
     <row r="679">
-      <c r="A679" s="13"/>
+      <c r="A679" s="15"/>
     </row>
     <row r="680">
-      <c r="A680" s="13"/>
+      <c r="A680" s="15"/>
     </row>
     <row r="681">
-      <c r="A681" s="13"/>
+      <c r="A681" s="15"/>
     </row>
     <row r="682">
-      <c r="A682" s="13"/>
+      <c r="A682" s="15"/>
     </row>
     <row r="683">
-      <c r="A683" s="13"/>
+      <c r="A683" s="15"/>
     </row>
     <row r="684">
-      <c r="A684" s="13"/>
+      <c r="A684" s="15"/>
     </row>
     <row r="685">
-      <c r="A685" s="13"/>
+      <c r="A685" s="15"/>
     </row>
     <row r="686">
-      <c r="A686" s="13"/>
+      <c r="A686" s="15"/>
     </row>
     <row r="687">
-      <c r="A687" s="13"/>
+      <c r="A687" s="15"/>
     </row>
     <row r="688">
-      <c r="A688" s="13"/>
+      <c r="A688" s="15"/>
     </row>
     <row r="689">
-      <c r="A689" s="13"/>
+      <c r="A689" s="15"/>
     </row>
     <row r="690">
-      <c r="A690" s="13"/>
+      <c r="A690" s="15"/>
     </row>
     <row r="691">
-      <c r="A691" s="13"/>
+      <c r="A691" s="15"/>
     </row>
     <row r="692">
-      <c r="A692" s="13"/>
+      <c r="A692" s="15"/>
     </row>
     <row r="693">
-      <c r="A693" s="13"/>
+      <c r="A693" s="15"/>
     </row>
     <row r="694">
-      <c r="A694" s="13"/>
+      <c r="A694" s="15"/>
     </row>
     <row r="695">
-      <c r="A695" s="13"/>
+      <c r="A695" s="15"/>
     </row>
     <row r="696">
-      <c r="A696" s="13"/>
+      <c r="A696" s="15"/>
     </row>
     <row r="697">
-      <c r="A697" s="13"/>
+      <c r="A697" s="15"/>
     </row>
     <row r="698">
-      <c r="A698" s="13"/>
+      <c r="A698" s="15"/>
     </row>
     <row r="699">
-      <c r="A699" s="13"/>
+      <c r="A699" s="15"/>
     </row>
     <row r="700">
-      <c r="A700" s="13"/>
+      <c r="A700" s="15"/>
     </row>
     <row r="701">
-      <c r="A701" s="13"/>
+      <c r="A701" s="15"/>
     </row>
     <row r="702">
-      <c r="A702" s="13"/>
+      <c r="A702" s="15"/>
     </row>
     <row r="703">
-      <c r="A703" s="13"/>
+      <c r="A703" s="15"/>
     </row>
     <row r="704">
-      <c r="A704" s="13"/>
+      <c r="A704" s="15"/>
     </row>
     <row r="705">
-      <c r="A705" s="13"/>
+      <c r="A705" s="15"/>
     </row>
     <row r="706">
-      <c r="A706" s="13"/>
+      <c r="A706" s="15"/>
     </row>
     <row r="707">
-      <c r="A707" s="13"/>
+      <c r="A707" s="15"/>
     </row>
     <row r="708">
-      <c r="A708" s="13"/>
+      <c r="A708" s="15"/>
     </row>
     <row r="709">
-      <c r="A709" s="13"/>
+      <c r="A709" s="15"/>
     </row>
     <row r="710">
-      <c r="A710" s="13"/>
+      <c r="A710" s="15"/>
     </row>
     <row r="711">
-      <c r="A711" s="13"/>
+      <c r="A711" s="15"/>
     </row>
     <row r="712">
-      <c r="A712" s="13"/>
+      <c r="A712" s="15"/>
     </row>
     <row r="713">
-      <c r="A713" s="13"/>
+      <c r="A713" s="15"/>
     </row>
     <row r="714">
-      <c r="A714" s="13"/>
+      <c r="A714" s="15"/>
     </row>
     <row r="715">
-      <c r="A715" s="13"/>
+      <c r="A715" s="15"/>
     </row>
     <row r="716">
-      <c r="A716" s="13"/>
+      <c r="A716" s="15"/>
     </row>
     <row r="717">
-      <c r="A717" s="13"/>
+      <c r="A717" s="15"/>
     </row>
     <row r="718">
-      <c r="A718" s="13"/>
+      <c r="A718" s="15"/>
     </row>
     <row r="719">
-      <c r="A719" s="13"/>
+      <c r="A719" s="15"/>
     </row>
     <row r="720">
-      <c r="A720" s="13"/>
+      <c r="A720" s="15"/>
     </row>
     <row r="721">
-      <c r="A721" s="13"/>
+      <c r="A721" s="15"/>
     </row>
     <row r="722">
-      <c r="A722" s="13"/>
+      <c r="A722" s="15"/>
     </row>
     <row r="723">
-      <c r="A723" s="13"/>
+      <c r="A723" s="15"/>
     </row>
     <row r="724">
-      <c r="A724" s="13"/>
+      <c r="A724" s="15"/>
     </row>
     <row r="725">
-      <c r="A725" s="13"/>
+      <c r="A725" s="15"/>
     </row>
     <row r="726">
-      <c r="A726" s="13"/>
+      <c r="A726" s="15"/>
     </row>
     <row r="727">
-      <c r="A727" s="13"/>
+      <c r="A727" s="15"/>
     </row>
     <row r="728">
-      <c r="A728" s="13"/>
+      <c r="A728" s="15"/>
     </row>
     <row r="729">
-      <c r="A729" s="13"/>
+      <c r="A729" s="15"/>
     </row>
     <row r="730">
-      <c r="A730" s="13"/>
+      <c r="A730" s="15"/>
     </row>
     <row r="731">
-      <c r="A731" s="13"/>
+      <c r="A731" s="15"/>
     </row>
     <row r="732">
-      <c r="A732" s="13"/>
+      <c r="A732" s="15"/>
     </row>
     <row r="733">
-      <c r="A733" s="13"/>
+      <c r="A733" s="15"/>
     </row>
     <row r="734">
-      <c r="A734" s="13"/>
+      <c r="A734" s="15"/>
     </row>
     <row r="735">
-      <c r="A735" s="13"/>
+      <c r="A735" s="15"/>
     </row>
     <row r="736">
-      <c r="A736" s="13"/>
+      <c r="A736" s="15"/>
     </row>
     <row r="737">
-      <c r="A737" s="13"/>
+      <c r="A737" s="15"/>
     </row>
     <row r="738">
-      <c r="A738" s="13"/>
+      <c r="A738" s="15"/>
     </row>
     <row r="739">
-      <c r="A739" s="13"/>
+      <c r="A739" s="15"/>
     </row>
     <row r="740">
-      <c r="A740" s="13"/>
+      <c r="A740" s="15"/>
     </row>
     <row r="741">
-      <c r="A741" s="13"/>
+      <c r="A741" s="15"/>
     </row>
     <row r="742">
-      <c r="A742" s="13"/>
+      <c r="A742" s="15"/>
     </row>
     <row r="743">
-      <c r="A743" s="13"/>
+      <c r="A743" s="15"/>
     </row>
     <row r="744">
-      <c r="A744" s="13"/>
+      <c r="A744" s="15"/>
     </row>
     <row r="745">
-      <c r="A745" s="13"/>
+      <c r="A745" s="15"/>
     </row>
     <row r="746">
-      <c r="A746" s="13"/>
+      <c r="A746" s="15"/>
     </row>
     <row r="747">
-      <c r="A747" s="13"/>
+      <c r="A747" s="15"/>
     </row>
     <row r="748">
-      <c r="A748" s="13"/>
+      <c r="A748" s="15"/>
     </row>
     <row r="749">
-      <c r="A749" s="13"/>
+      <c r="A749" s="15"/>
     </row>
     <row r="750">
-      <c r="A750" s="13"/>
+      <c r="A750" s="15"/>
     </row>
     <row r="751">
-      <c r="A751" s="13"/>
+      <c r="A751" s="15"/>
     </row>
     <row r="752">
-      <c r="A752" s="13"/>
+      <c r="A752" s="15"/>
     </row>
     <row r="753">
-      <c r="A753" s="13"/>
+      <c r="A753" s="15"/>
     </row>
     <row r="754">
-      <c r="A754" s="13"/>
+      <c r="A754" s="15"/>
     </row>
     <row r="755">
-      <c r="A755" s="13"/>
+      <c r="A755" s="15"/>
     </row>
     <row r="756">
-      <c r="A756" s="13"/>
+      <c r="A756" s="15"/>
     </row>
     <row r="757">
-      <c r="A757" s="13"/>
+      <c r="A757" s="15"/>
     </row>
     <row r="758">
-      <c r="A758" s="13"/>
+      <c r="A758" s="15"/>
     </row>
     <row r="759">
-      <c r="A759" s="13"/>
+      <c r="A759" s="15"/>
     </row>
     <row r="760">
-      <c r="A760" s="13"/>
+      <c r="A760" s="15"/>
     </row>
     <row r="761">
-      <c r="A761" s="13"/>
+      <c r="A761" s="15"/>
     </row>
     <row r="762">
-      <c r="A762" s="13"/>
+      <c r="A762" s="15"/>
     </row>
     <row r="763">
-      <c r="A763" s="13"/>
+      <c r="A763" s="15"/>
     </row>
     <row r="764">
-      <c r="A764" s="13"/>
+      <c r="A764" s="15"/>
     </row>
     <row r="765">
-      <c r="A765" s="13"/>
+      <c r="A765" s="15"/>
     </row>
     <row r="766">
-      <c r="A766" s="13"/>
+      <c r="A766" s="15"/>
     </row>
     <row r="767">
-      <c r="A767" s="13"/>
+      <c r="A767" s="15"/>
     </row>
     <row r="768">
-      <c r="A768" s="13"/>
+      <c r="A768" s="15"/>
     </row>
     <row r="769">
-      <c r="A769" s="13"/>
+      <c r="A769" s="15"/>
     </row>
     <row r="770">
-      <c r="A770" s="13"/>
+      <c r="A770" s="15"/>
     </row>
     <row r="771">
-      <c r="A771" s="13"/>
+      <c r="A771" s="15"/>
     </row>
     <row r="772">
-      <c r="A772" s="13"/>
+      <c r="A772" s="15"/>
     </row>
     <row r="773">
-      <c r="A773" s="13"/>
+      <c r="A773" s="15"/>
     </row>
     <row r="774">
-      <c r="A774" s="13"/>
+      <c r="A774" s="15"/>
     </row>
     <row r="775">
-      <c r="A775" s="13"/>
+      <c r="A775" s="15"/>
     </row>
     <row r="776">
-      <c r="A776" s="13"/>
+      <c r="A776" s="15"/>
     </row>
     <row r="777">
-      <c r="A777" s="13"/>
+      <c r="A777" s="15"/>
     </row>
     <row r="778">
-      <c r="A778" s="13"/>
+      <c r="A778" s="15"/>
     </row>
     <row r="779">
-      <c r="A779" s="13"/>
+      <c r="A779" s="15"/>
     </row>
     <row r="780">
-      <c r="A780" s="13"/>
+      <c r="A780" s="15"/>
     </row>
     <row r="781">
-      <c r="A781" s="13"/>
+      <c r="A781" s="15"/>
     </row>
     <row r="782">
-      <c r="A782" s="13"/>
+      <c r="A782" s="15"/>
     </row>
     <row r="783">
-      <c r="A783" s="13"/>
+      <c r="A783" s="15"/>
     </row>
     <row r="784">
-      <c r="A784" s="13"/>
+      <c r="A784" s="15"/>
     </row>
     <row r="785">
-      <c r="A785" s="13"/>
+      <c r="A785" s="15"/>
     </row>
     <row r="786">
-      <c r="A786" s="13"/>
+      <c r="A786" s="15"/>
     </row>
     <row r="787">
-      <c r="A787" s="13"/>
+      <c r="A787" s="15"/>
     </row>
     <row r="788">
-      <c r="A788" s="13"/>
+      <c r="A788" s="15"/>
     </row>
     <row r="789">
-      <c r="A789" s="13"/>
+      <c r="A789" s="15"/>
     </row>
     <row r="790">
-      <c r="A790" s="13"/>
+      <c r="A790" s="15"/>
     </row>
     <row r="791">
-      <c r="A791" s="13"/>
+      <c r="A791" s="15"/>
     </row>
     <row r="792">
-      <c r="A792" s="13"/>
+      <c r="A792" s="15"/>
     </row>
     <row r="793">
-      <c r="A793" s="13"/>
+      <c r="A793" s="15"/>
     </row>
     <row r="794">
-      <c r="A794" s="13"/>
+      <c r="A794" s="15"/>
     </row>
     <row r="795">
-      <c r="A795" s="13"/>
+      <c r="A795" s="15"/>
     </row>
     <row r="796">
-      <c r="A796" s="13"/>
+      <c r="A796" s="15"/>
     </row>
     <row r="797">
-      <c r="A797" s="13"/>
+      <c r="A797" s="15"/>
     </row>
     <row r="798">
-      <c r="A798" s="13"/>
+      <c r="A798" s="15"/>
     </row>
     <row r="799">
-      <c r="A799" s="13"/>
+      <c r="A799" s="15"/>
     </row>
     <row r="800">
-      <c r="A800" s="13"/>
+      <c r="A800" s="15"/>
     </row>
     <row r="801">
-      <c r="A801" s="13"/>
+      <c r="A801" s="15"/>
     </row>
     <row r="802">
-      <c r="A802" s="13"/>
+      <c r="A802" s="15"/>
     </row>
     <row r="803">
-      <c r="A803" s="13"/>
+      <c r="A803" s="15"/>
     </row>
     <row r="804">
-      <c r="A804" s="13"/>
+      <c r="A804" s="15"/>
     </row>
     <row r="805">
-      <c r="A805" s="13"/>
+      <c r="A805" s="15"/>
     </row>
     <row r="806">
-      <c r="A806" s="13"/>
+      <c r="A806" s="15"/>
     </row>
     <row r="807">
-      <c r="A807" s="13"/>
+      <c r="A807" s="15"/>
     </row>
     <row r="808">
-      <c r="A808" s="13"/>
+      <c r="A808" s="15"/>
     </row>
     <row r="809">
-      <c r="A809" s="13"/>
+      <c r="A809" s="15"/>
     </row>
     <row r="810">
-      <c r="A810" s="13"/>
+      <c r="A810" s="15"/>
     </row>
     <row r="811">
-      <c r="A811" s="13"/>
+      <c r="A811" s="15"/>
     </row>
     <row r="812">
-      <c r="A812" s="13"/>
+      <c r="A812" s="15"/>
     </row>
     <row r="813">
-      <c r="A813" s="13"/>
+      <c r="A813" s="15"/>
     </row>
     <row r="814">
-      <c r="A814" s="13"/>
+      <c r="A814" s="15"/>
     </row>
     <row r="815">
-      <c r="A815" s="13"/>
+      <c r="A815" s="15"/>
     </row>
     <row r="816">
-      <c r="A816" s="13"/>
+      <c r="A816" s="15"/>
     </row>
     <row r="817">
-      <c r="A817" s="13"/>
+      <c r="A817" s="15"/>
     </row>
     <row r="818">
-      <c r="A818" s="13"/>
+      <c r="A818" s="15"/>
     </row>
     <row r="819">
-      <c r="A819" s="13"/>
+      <c r="A819" s="15"/>
     </row>
     <row r="820">
-      <c r="A820" s="13"/>
+      <c r="A820" s="15"/>
     </row>
     <row r="821">
-      <c r="A821" s="13"/>
+      <c r="A821" s="15"/>
     </row>
     <row r="822">
-      <c r="A822" s="13"/>
+      <c r="A822" s="15"/>
     </row>
     <row r="823">
-      <c r="A823" s="13"/>
+      <c r="A823" s="15"/>
     </row>
     <row r="824">
-      <c r="A824" s="13"/>
+      <c r="A824" s="15"/>
     </row>
     <row r="825">
-      <c r="A825" s="13"/>
+      <c r="A825" s="15"/>
     </row>
     <row r="826">
-      <c r="A826" s="13"/>
+      <c r="A826" s="15"/>
     </row>
     <row r="827">
-      <c r="A827" s="13"/>
+      <c r="A827" s="15"/>
     </row>
     <row r="828">
-      <c r="A828" s="13"/>
+      <c r="A828" s="15"/>
     </row>
     <row r="829">
-      <c r="A829" s="13"/>
+      <c r="A829" s="15"/>
     </row>
     <row r="830">
-      <c r="A830" s="13"/>
+      <c r="A830" s="15"/>
     </row>
     <row r="831">
-      <c r="A831" s="13"/>
+      <c r="A831" s="15"/>
     </row>
     <row r="832">
-      <c r="A832" s="13"/>
+      <c r="A832" s="15"/>
     </row>
     <row r="833">
-      <c r="A833" s="13"/>
+      <c r="A833" s="15"/>
     </row>
     <row r="834">
-      <c r="A834" s="13"/>
+      <c r="A834" s="15"/>
     </row>
     <row r="835">
-      <c r="A835" s="13"/>
+      <c r="A835" s="15"/>
     </row>
     <row r="836">
-      <c r="A836" s="13"/>
+      <c r="A836" s="15"/>
     </row>
     <row r="837">
-      <c r="A837" s="13"/>
+      <c r="A837" s="15"/>
     </row>
     <row r="838">
-      <c r="A838" s="13"/>
+      <c r="A838" s="15"/>
     </row>
     <row r="839">
-      <c r="A839" s="13"/>
+      <c r="A839" s="15"/>
     </row>
     <row r="840">
-      <c r="A840" s="13"/>
+      <c r="A840" s="15"/>
     </row>
     <row r="841">
-      <c r="A841" s="13"/>
+      <c r="A841" s="15"/>
     </row>
     <row r="842">
-      <c r="A842" s="13"/>
+      <c r="A842" s="15"/>
     </row>
     <row r="843">
-      <c r="A843" s="13"/>
+      <c r="A843" s="15"/>
     </row>
     <row r="844">
-      <c r="A844" s="13"/>
+      <c r="A844" s="15"/>
     </row>
     <row r="845">
-      <c r="A845" s="13"/>
+      <c r="A845" s="15"/>
     </row>
     <row r="846">
-      <c r="A846" s="13"/>
+      <c r="A846" s="15"/>
     </row>
     <row r="847">
-      <c r="A847" s="13"/>
+      <c r="A847" s="15"/>
     </row>
     <row r="848">
-      <c r="A848" s="13"/>
+      <c r="A848" s="15"/>
     </row>
     <row r="849">
-      <c r="A849" s="13"/>
+      <c r="A849" s="15"/>
     </row>
     <row r="850">
-      <c r="A850" s="13"/>
+      <c r="A850" s="15"/>
     </row>
     <row r="851">
-      <c r="A851" s="13"/>
+      <c r="A851" s="15"/>
     </row>
     <row r="852">
-      <c r="A852" s="13"/>
+      <c r="A852" s="15"/>
     </row>
     <row r="853">
-      <c r="A853" s="13"/>
+      <c r="A853" s="15"/>
     </row>
     <row r="854">
-      <c r="A854" s="13"/>
+      <c r="A854" s="15"/>
     </row>
     <row r="855">
-      <c r="A855" s="13"/>
+      <c r="A855" s="15"/>
     </row>
     <row r="856">
-      <c r="A856" s="13"/>
+      <c r="A856" s="15"/>
     </row>
     <row r="857">
-      <c r="A857" s="13"/>
+      <c r="A857" s="15"/>
     </row>
     <row r="858">
-      <c r="A858" s="13"/>
+      <c r="A858" s="15"/>
     </row>
     <row r="859">
-      <c r="A859" s="13"/>
+      <c r="A859" s="15"/>
     </row>
     <row r="860">
-      <c r="A860" s="13"/>
+      <c r="A860" s="15"/>
     </row>
     <row r="861">
-      <c r="A861" s="13"/>
+      <c r="A861" s="15"/>
     </row>
     <row r="862">
-      <c r="A862" s="13"/>
+      <c r="A862" s="15"/>
     </row>
     <row r="863">
-      <c r="A863" s="13"/>
+      <c r="A863" s="15"/>
     </row>
     <row r="864">
-      <c r="A864" s="13"/>
+      <c r="A864" s="15"/>
     </row>
     <row r="865">
-      <c r="A865" s="13"/>
+      <c r="A865" s="15"/>
     </row>
     <row r="866">
-      <c r="A866" s="13"/>
+      <c r="A866" s="15"/>
     </row>
     <row r="867">
-      <c r="A867" s="13"/>
+      <c r="A867" s="15"/>
     </row>
     <row r="868">
-      <c r="A868" s="13"/>
+      <c r="A868" s="15"/>
     </row>
     <row r="869">
-      <c r="A869" s="13"/>
+      <c r="A869" s="15"/>
     </row>
     <row r="870">
-      <c r="A870" s="13"/>
+      <c r="A870" s="15"/>
     </row>
     <row r="871">
-      <c r="A871" s="13"/>
+      <c r="A871" s="15"/>
     </row>
     <row r="872">
-      <c r="A872" s="13"/>
+      <c r="A872" s="15"/>
     </row>
     <row r="873">
-      <c r="A873" s="13"/>
+      <c r="A873" s="15"/>
     </row>
     <row r="874">
-      <c r="A874" s="13"/>
+      <c r="A874" s="15"/>
     </row>
     <row r="875">
-      <c r="A875" s="13"/>
+      <c r="A875" s="15"/>
     </row>
     <row r="876">
-      <c r="A876" s="13"/>
+      <c r="A876" s="15"/>
     </row>
     <row r="877">
-      <c r="A877" s="13"/>
+      <c r="A877" s="15"/>
     </row>
     <row r="878">
-      <c r="A878" s="13"/>
+      <c r="A878" s="15"/>
     </row>
     <row r="879">
-      <c r="A879" s="13"/>
+      <c r="A879" s="15"/>
     </row>
     <row r="880">
-      <c r="A880" s="13"/>
+      <c r="A880" s="15"/>
     </row>
     <row r="881">
-      <c r="A881" s="13"/>
+      <c r="A881" s="15"/>
     </row>
     <row r="882">
-      <c r="A882" s="13"/>
+      <c r="A882" s="15"/>
     </row>
     <row r="883">
-      <c r="A883" s="13"/>
+      <c r="A883" s="15"/>
     </row>
     <row r="884">
-      <c r="A884" s="13"/>
+      <c r="A884" s="15"/>
     </row>
     <row r="885">
-      <c r="A885" s="13"/>
+      <c r="A885" s="15"/>
     </row>
     <row r="886">
-      <c r="A886" s="13"/>
+      <c r="A886" s="15"/>
     </row>
     <row r="887">
-      <c r="A887" s="13"/>
+      <c r="A887" s="15"/>
     </row>
     <row r="888">
-      <c r="A888" s="13"/>
+      <c r="A888" s="15"/>
     </row>
     <row r="889">
-      <c r="A889" s="13"/>
+      <c r="A889" s="15"/>
     </row>
     <row r="890">
-      <c r="A890" s="13"/>
+      <c r="A890" s="15"/>
     </row>
     <row r="891">
-      <c r="A891" s="13"/>
+      <c r="A891" s="15"/>
     </row>
     <row r="892">
-      <c r="A892" s="13"/>
+      <c r="A892" s="15"/>
     </row>
     <row r="893">
-      <c r="A893" s="13"/>
+      <c r="A893" s="15"/>
     </row>
     <row r="894">
-      <c r="A894" s="13"/>
+      <c r="A894" s="15"/>
     </row>
     <row r="895">
-      <c r="A895" s="13"/>
+      <c r="A895" s="15"/>
     </row>
     <row r="896">
-      <c r="A896" s="13"/>
+      <c r="A896" s="15"/>
     </row>
     <row r="897">
-      <c r="A897" s="13"/>
+      <c r="A897" s="15"/>
     </row>
     <row r="898">
-      <c r="A898" s="13"/>
+      <c r="A898" s="15"/>
     </row>
     <row r="899">
-      <c r="A899" s="13"/>
+      <c r="A899" s="15"/>
     </row>
     <row r="900">
-      <c r="A900" s="13"/>
+      <c r="A900" s="15"/>
     </row>
     <row r="901">
-      <c r="A901" s="13"/>
+      <c r="A901" s="15"/>
     </row>
     <row r="902">
-      <c r="A902" s="13"/>
+      <c r="A902" s="15"/>
     </row>
     <row r="903">
-      <c r="A903" s="13"/>
+      <c r="A903" s="15"/>
     </row>
     <row r="904">
-      <c r="A904" s="13"/>
+      <c r="A904" s="15"/>
     </row>
     <row r="905">
-      <c r="A905" s="13"/>
+      <c r="A905" s="15"/>
     </row>
     <row r="906">
-      <c r="A906" s="13"/>
+      <c r="A906" s="15"/>
     </row>
     <row r="907">
-      <c r="A907" s="13"/>
+      <c r="A907" s="15"/>
     </row>
     <row r="908">
-      <c r="A908" s="13"/>
+      <c r="A908" s="15"/>
     </row>
     <row r="909">
-      <c r="A909" s="13"/>
+      <c r="A909" s="15"/>
     </row>
     <row r="910">
-      <c r="A910" s="13"/>
+      <c r="A910" s="15"/>
     </row>
     <row r="911">
-      <c r="A911" s="13"/>
+      <c r="A911" s="15"/>
     </row>
     <row r="912">
-      <c r="A912" s="13"/>
+      <c r="A912" s="15"/>
     </row>
     <row r="913">
-      <c r="A913" s="13"/>
+      <c r="A913" s="15"/>
     </row>
     <row r="914">
-      <c r="A914" s="13"/>
+      <c r="A914" s="15"/>
     </row>
     <row r="915">
-      <c r="A915" s="13"/>
+      <c r="A915" s="15"/>
     </row>
     <row r="916">
-      <c r="A916" s="13"/>
+      <c r="A916" s="15"/>
     </row>
     <row r="917">
-      <c r="A917" s="13"/>
+      <c r="A917" s="15"/>
     </row>
     <row r="918">
-      <c r="A918" s="13"/>
+      <c r="A918" s="15"/>
     </row>
     <row r="919">
-      <c r="A919" s="13"/>
+      <c r="A919" s="15"/>
     </row>
     <row r="920">
-      <c r="A920" s="13"/>
+      <c r="A920" s="15"/>
     </row>
     <row r="921">
-      <c r="A921" s="13"/>
+      <c r="A921" s="15"/>
     </row>
     <row r="922">
-      <c r="A922" s="13"/>
+      <c r="A922" s="15"/>
     </row>
     <row r="923">
-      <c r="A923" s="13"/>
+      <c r="A923" s="15"/>
     </row>
     <row r="924">
-      <c r="A924" s="13"/>
+      <c r="A924" s="15"/>
     </row>
     <row r="925">
-      <c r="A925" s="13"/>
+      <c r="A925" s="15"/>
     </row>
     <row r="926">
-      <c r="A926" s="13"/>
+      <c r="A926" s="15"/>
     </row>
     <row r="927">
-      <c r="A927" s="13"/>
+      <c r="A927" s="15"/>
     </row>
     <row r="928">
-      <c r="A928" s="13"/>
+      <c r="A928" s="15"/>
     </row>
     <row r="929">
-      <c r="A929" s="13"/>
+      <c r="A929" s="15"/>
     </row>
     <row r="930">
-      <c r="A930" s="13"/>
+      <c r="A930" s="15"/>
     </row>
     <row r="931">
-      <c r="A931" s="13"/>
+      <c r="A931" s="15"/>
     </row>
     <row r="932">
-      <c r="A932" s="13"/>
+      <c r="A932" s="15"/>
     </row>
     <row r="933">
-      <c r="A933" s="13"/>
+      <c r="A933" s="15"/>
     </row>
     <row r="934">
-      <c r="A934" s="13"/>
+      <c r="A934" s="15"/>
     </row>
     <row r="935">
-      <c r="A935" s="13"/>
+      <c r="A935" s="15"/>
     </row>
     <row r="936">
-      <c r="A936" s="13"/>
+      <c r="A936" s="15"/>
     </row>
     <row r="937">
-      <c r="A937" s="13"/>
+      <c r="A937" s="15"/>
     </row>
     <row r="938">
-      <c r="A938" s="13"/>
+      <c r="A938" s="15"/>
     </row>
     <row r="939">
-      <c r="A939" s="13"/>
+      <c r="A939" s="15"/>
     </row>
     <row r="940">
-      <c r="A940" s="13"/>
+      <c r="A940" s="15"/>
     </row>
     <row r="941">
-      <c r="A941" s="13"/>
+      <c r="A941" s="15"/>
     </row>
     <row r="942">
-      <c r="A942" s="13"/>
+      <c r="A942" s="15"/>
     </row>
     <row r="943">
-      <c r="A943" s="13"/>
+      <c r="A943" s="15"/>
     </row>
     <row r="944">
-      <c r="A944" s="13"/>
+      <c r="A944" s="15"/>
     </row>
     <row r="945">
-      <c r="A945" s="13"/>
+      <c r="A945" s="15"/>
     </row>
     <row r="946">
-      <c r="A946" s="13"/>
+      <c r="A946" s="15"/>
     </row>
     <row r="947">
-      <c r="A947" s="13"/>
+      <c r="A947" s="15"/>
     </row>
     <row r="948">
-      <c r="A948" s="13"/>
+      <c r="A948" s="15"/>
     </row>
     <row r="949">
-      <c r="A949" s="13"/>
+      <c r="A949" s="15"/>
     </row>
     <row r="950">
-      <c r="A950" s="13"/>
+      <c r="A950" s="15"/>
     </row>
     <row r="951">
-      <c r="A951" s="13"/>
+      <c r="A951" s="15"/>
     </row>
     <row r="952">
-      <c r="A952" s="13"/>
+      <c r="A952" s="15"/>
     </row>
     <row r="953">
-      <c r="A953" s="13"/>
+      <c r="A953" s="15"/>
     </row>
     <row r="954">
-      <c r="A954" s="13"/>
+      <c r="A954" s="15"/>
     </row>
     <row r="955">
-      <c r="A955" s="13"/>
+      <c r="A955" s="15"/>
     </row>
     <row r="956">
-      <c r="A956" s="13"/>
+      <c r="A956" s="15"/>
     </row>
     <row r="957">
-      <c r="A957" s="13"/>
+      <c r="A957" s="15"/>
     </row>
     <row r="958">
-      <c r="A958" s="13"/>
+      <c r="A958" s="15"/>
     </row>
     <row r="959">
-      <c r="A959" s="13"/>
+      <c r="A959" s="15"/>
     </row>
     <row r="960">
-      <c r="A960" s="13"/>
+      <c r="A960" s="15"/>
     </row>
     <row r="961">
-      <c r="A961" s="13"/>
+      <c r="A961" s="15"/>
     </row>
     <row r="962">
-      <c r="A962" s="13"/>
+      <c r="A962" s="15"/>
     </row>
     <row r="963">
-      <c r="A963" s="13"/>
+      <c r="A963" s="15"/>
     </row>
     <row r="964">
-      <c r="A964" s="13"/>
+      <c r="A964" s="15"/>
     </row>
     <row r="965">
-      <c r="A965" s="13"/>
+      <c r="A965" s="15"/>
     </row>
     <row r="966">
-      <c r="A966" s="13"/>
+      <c r="A966" s="15"/>
     </row>
     <row r="967">
-      <c r="A967" s="13"/>
+      <c r="A967" s="15"/>
     </row>
     <row r="968">
-      <c r="A968" s="13"/>
+      <c r="A968" s="15"/>
     </row>
     <row r="969">
-      <c r="A969" s="13"/>
+      <c r="A969" s="15"/>
     </row>
     <row r="970">
-      <c r="A970" s="13"/>
+      <c r="A970" s="15"/>
     </row>
     <row r="971">
-      <c r="A971" s="13"/>
+      <c r="A971" s="15"/>
     </row>
     <row r="972">
-      <c r="A972" s="13"/>
+      <c r="A972" s="15"/>
     </row>
     <row r="973">
-      <c r="A973" s="13"/>
+      <c r="A973" s="15"/>
     </row>
     <row r="974">
-      <c r="A974" s="13"/>
+      <c r="A974" s="15"/>
     </row>
     <row r="975">
-      <c r="A975" s="13"/>
+      <c r="A975" s="15"/>
     </row>
     <row r="976">
-      <c r="A976" s="13"/>
+      <c r="A976" s="15"/>
     </row>
     <row r="977">
-      <c r="A977" s="13"/>
+      <c r="A977" s="15"/>
     </row>
     <row r="978">
-      <c r="A978" s="13"/>
+      <c r="A978" s="15"/>
     </row>
     <row r="979">
-      <c r="A979" s="13"/>
+      <c r="A979" s="15"/>
     </row>
     <row r="980">
-      <c r="A980" s="13"/>
+      <c r="A980" s="15"/>
     </row>
     <row r="981">
-      <c r="A981" s="13"/>
+      <c r="A981" s="15"/>
     </row>
     <row r="982">
-      <c r="A982" s="13"/>
+      <c r="A982" s="15"/>
     </row>
     <row r="983">
-      <c r="A983" s="13"/>
+      <c r="A983" s="15"/>
     </row>
     <row r="984">
-      <c r="A984" s="13"/>
+      <c r="A984" s="15"/>
     </row>
     <row r="985">
-      <c r="A985" s="13"/>
+      <c r="A985" s="15"/>
     </row>
     <row r="986">
-      <c r="A986" s="13"/>
+      <c r="A986" s="15"/>
     </row>
     <row r="987">
-      <c r="A987" s="13"/>
+      <c r="A987" s="15"/>
     </row>
     <row r="988">
-      <c r="A988" s="13"/>
+      <c r="A988" s="15"/>
     </row>
     <row r="989">
-      <c r="A989" s="13"/>
+      <c r="A989" s="15"/>
     </row>
     <row r="990">
-      <c r="A990" s="13"/>
+      <c r="A990" s="15"/>
     </row>
     <row r="991">
-      <c r="A991" s="13"/>
+      <c r="A991" s="15"/>
     </row>
     <row r="992">
-      <c r="A992" s="13"/>
+      <c r="A992" s="15"/>
     </row>
     <row r="993">
-      <c r="A993" s="13"/>
+      <c r="A993" s="15"/>
     </row>
     <row r="994">
-      <c r="A994" s="13"/>
+      <c r="A994" s="15"/>
     </row>
     <row r="995">
-      <c r="A995" s="13"/>
+      <c r="A995" s="15"/>
     </row>
     <row r="996">
-      <c r="A996" s="13"/>
+      <c r="A996" s="15"/>
     </row>
     <row r="997">
-      <c r="A997" s="13"/>
+      <c r="A997" s="15"/>
     </row>
     <row r="998">
-      <c r="A998" s="13"/>
+      <c r="A998" s="15"/>
     </row>
     <row r="999">
-      <c r="A999" s="13"/>
+      <c r="A999" s="15"/>
     </row>
     <row r="1000">
-      <c r="A1000" s="13"/>
+      <c r="A1000" s="15"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -10046,7 +10174,7 @@
         <v>9</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>11</v>
@@ -10151,7 +10279,7 @@
         <v>44</v>
       </c>
       <c r="AS2" s="12" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="AT2" s="12" t="s">
         <v>46</v>
@@ -10642,67 +10770,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -10725,7 +10853,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2">
@@ -10735,42 +10863,42 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -10793,12 +10921,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -10820,93 +10948,93 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
-        <v>258</v>
+      <c r="A1" s="16" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="12" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>